<commit_message>
Avance 16 de junio
</commit_message>
<xml_diff>
--- a/Proyecto Final/Costos proyecto ensayos.xlsx
+++ b/Proyecto Final/Costos proyecto ensayos.xlsx
@@ -196,7 +196,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="184" formatCode="_-&quot;$&quot;\ * #,##0.000000000000000000000_-;\-&quot;$&quot;\ * #,##0.000000000000000000000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.000000000000000000000_-;\-&quot;$&quot;\ * #,##0.000000000000000000000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -368,7 +368,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -394,6 +394,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,15 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -774,7 +775,7 @@
   <dimension ref="B1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,34 +790,35 @@
     <col min="10" max="10" width="19" style="6" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.5546875" style="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.88671875" customWidth="1"/>
-    <col min="20" max="20" width="12.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.77734375" style="16" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-      <c r="J2" s="15" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="J2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="17"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="26"/>
       <c r="U2" s="11" t="s">
         <v>28</v>
       </c>
@@ -861,7 +863,7 @@
       <c r="N3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="P3" s="4" t="s">
@@ -902,27 +904,31 @@
       <c r="J4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <f>O4*L4</f>
         <v>43853908.125649996</v>
       </c>
-      <c r="L4" s="25">
-        <v>25</v>
-      </c>
-      <c r="M4" s="25">
-        <v>8</v>
-      </c>
-      <c r="N4" s="25">
+      <c r="L4" s="22">
+        <v>25</v>
+      </c>
+      <c r="M4" s="22">
+        <v>8</v>
+      </c>
+      <c r="N4" s="22">
         <f>+M4*L4</f>
         <v>200</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="19">
         <f>P4*M4</f>
         <v>1754156.3250259999</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="19">
         <f>291550*R5</f>
         <v>219269.54062824999</v>
+      </c>
+      <c r="Q4" s="27">
+        <f>P4*40</f>
+        <v>8770781.6251299996</v>
       </c>
       <c r="U4" s="13" t="s">
         <v>32</v>
@@ -959,25 +965,25 @@
       <c r="J5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="22">
         <f t="shared" ref="K5:K16" si="3">O5*L5</f>
         <v>35620113.130630001</v>
       </c>
-      <c r="L5" s="25">
-        <v>25</v>
-      </c>
-      <c r="M5" s="25">
-        <v>8</v>
-      </c>
-      <c r="N5" s="25">
+      <c r="L5" s="22">
+        <v>25</v>
+      </c>
+      <c r="M5" s="22">
+        <v>8</v>
+      </c>
+      <c r="N5" s="22">
         <f t="shared" ref="N5:N16" si="4">+M5*L5</f>
         <v>200</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="19">
         <f t="shared" ref="O5:O16" si="5">P5*M5</f>
         <v>1424804.5252252</v>
       </c>
-      <c r="P5" s="22">
+      <c r="P5" s="19">
         <f>236810*R5</f>
         <v>178100.56565315</v>
       </c>
@@ -1016,25 +1022,25 @@
       <c r="J6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <f t="shared" si="3"/>
         <v>31324220.089749999</v>
       </c>
-      <c r="L6" s="25">
-        <v>25</v>
-      </c>
-      <c r="M6" s="25">
-        <v>8</v>
-      </c>
-      <c r="N6" s="25">
+      <c r="L6" s="22">
+        <v>25</v>
+      </c>
+      <c r="M6" s="22">
+        <v>8</v>
+      </c>
+      <c r="N6" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="19">
         <f t="shared" si="5"/>
         <v>1252968.8035899999</v>
       </c>
-      <c r="P6" s="22">
+      <c r="P6" s="19">
         <f>208250*R5</f>
         <v>156621.10044874999</v>
       </c>
@@ -1067,25 +1073,25 @@
       <c r="J7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="22">
         <f t="shared" si="3"/>
         <v>48149801.166529998</v>
       </c>
-      <c r="L7" s="25">
-        <v>25</v>
-      </c>
-      <c r="M7" s="25">
-        <v>8</v>
-      </c>
-      <c r="N7" s="25">
+      <c r="L7" s="22">
+        <v>25</v>
+      </c>
+      <c r="M7" s="22">
+        <v>8</v>
+      </c>
+      <c r="N7" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O7" s="22">
+      <c r="O7" s="19">
         <f t="shared" si="5"/>
         <v>1925992.0466612</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="19">
         <f>320110*R5</f>
         <v>240749.00583265</v>
       </c>
@@ -1118,25 +1124,25 @@
       <c r="J8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="22">
         <f t="shared" si="3"/>
         <v>48149801.166529998</v>
       </c>
-      <c r="L8" s="25">
-        <v>25</v>
-      </c>
-      <c r="M8" s="25">
-        <v>8</v>
-      </c>
-      <c r="N8" s="25">
+      <c r="L8" s="22">
+        <v>25</v>
+      </c>
+      <c r="M8" s="22">
+        <v>8</v>
+      </c>
+      <c r="N8" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O8" s="22">
+      <c r="O8" s="19">
         <f t="shared" si="5"/>
         <v>1925992.0466612</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="19">
         <f>320110*R5</f>
         <v>240749.00583265</v>
       </c>
@@ -1169,25 +1175,25 @@
       <c r="J9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="22">
         <f t="shared" si="3"/>
         <v>37231073.020960003</v>
       </c>
-      <c r="L9" s="25">
-        <v>25</v>
-      </c>
-      <c r="M9" s="25">
-        <v>8</v>
-      </c>
-      <c r="N9" s="25">
+      <c r="L9" s="22">
+        <v>25</v>
+      </c>
+      <c r="M9" s="22">
+        <v>8</v>
+      </c>
+      <c r="N9" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O9" s="22">
+      <c r="O9" s="19">
         <f t="shared" si="5"/>
         <v>1489242.9208384</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="19">
         <f>247520*R5</f>
         <v>186155.3651048</v>
       </c>
@@ -1220,29 +1226,29 @@
       <c r="J10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="22">
         <f t="shared" si="3"/>
         <v>48149801.166529998</v>
       </c>
-      <c r="L10" s="25">
-        <v>25</v>
-      </c>
-      <c r="M10" s="25">
-        <v>8</v>
-      </c>
-      <c r="N10" s="25">
+      <c r="L10" s="22">
+        <v>25</v>
+      </c>
+      <c r="M10" s="22">
+        <v>8</v>
+      </c>
+      <c r="N10" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="19">
         <f t="shared" si="5"/>
         <v>1925992.0466612</v>
       </c>
-      <c r="P10" s="22">
+      <c r="P10" s="19">
         <f>320110*R5</f>
         <v>240749.00583265</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="T10" s="16" t="s">
         <v>47</v>
       </c>
       <c r="U10" t="s">
@@ -1280,36 +1286,36 @@
       <c r="J11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="22">
         <f t="shared" si="3"/>
         <v>48149801.166529998</v>
       </c>
-      <c r="L11" s="25">
-        <v>25</v>
-      </c>
-      <c r="M11" s="25">
-        <v>8</v>
-      </c>
-      <c r="N11" s="25">
+      <c r="L11" s="22">
+        <v>25</v>
+      </c>
+      <c r="M11" s="22">
+        <v>8</v>
+      </c>
+      <c r="N11" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="19">
         <f t="shared" si="5"/>
         <v>1925992.0466612</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="19">
         <f>320110*R5</f>
         <v>240749.00583265</v>
       </c>
-      <c r="T11" s="19">
+      <c r="T11" s="16">
         <v>291550</v>
       </c>
-      <c r="U11" s="20">
+      <c r="U11" s="17">
         <f>T11*8</f>
         <v>2332400</v>
       </c>
-      <c r="V11" s="20">
+      <c r="V11" s="17">
         <f>U11*25</f>
         <v>58310000</v>
       </c>
@@ -1342,36 +1348,36 @@
       <c r="J12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="22">
         <f t="shared" si="3"/>
         <v>17183572.163520001</v>
       </c>
-      <c r="L12" s="25">
-        <v>25</v>
-      </c>
-      <c r="M12" s="25">
-        <v>8</v>
-      </c>
-      <c r="N12" s="25">
+      <c r="L12" s="22">
+        <v>25</v>
+      </c>
+      <c r="M12" s="22">
+        <v>8</v>
+      </c>
+      <c r="N12" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="19">
         <f t="shared" si="5"/>
         <v>687342.88654079998</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="19">
         <f>114240*R5</f>
         <v>85917.860817599998</v>
       </c>
-      <c r="T12" s="19">
+      <c r="T12" s="16">
         <v>236810</v>
       </c>
-      <c r="U12" s="20">
+      <c r="U12" s="17">
         <f>T12*8</f>
         <v>1894480</v>
       </c>
-      <c r="V12" s="20">
+      <c r="V12" s="17">
         <f>U12*25</f>
         <v>47362000</v>
       </c>
@@ -1402,36 +1408,36 @@
       <c r="J13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="22">
         <f t="shared" si="3"/>
         <v>18794532.053849999</v>
       </c>
-      <c r="L13" s="25">
-        <v>25</v>
-      </c>
-      <c r="M13" s="25">
-        <v>8</v>
-      </c>
-      <c r="N13" s="25">
+      <c r="L13" s="22">
+        <v>25</v>
+      </c>
+      <c r="M13" s="22">
+        <v>8</v>
+      </c>
+      <c r="N13" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="19">
         <f t="shared" si="5"/>
         <v>751781.28215400001</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="19">
         <f>124950*R5</f>
         <v>93972.660269250002</v>
       </c>
-      <c r="T13" s="19">
+      <c r="T13" s="16">
         <v>208250</v>
       </c>
-      <c r="U13" s="20">
+      <c r="U13" s="17">
         <f t="shared" ref="U13:U23" si="6">T13*8</f>
         <v>1666000</v>
       </c>
-      <c r="V13" s="20">
+      <c r="V13" s="17">
         <f t="shared" ref="V13:V23" si="7">U13*25</f>
         <v>41650000</v>
       </c>
@@ -1462,36 +1468,36 @@
       <c r="J14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="22">
         <f t="shared" si="3"/>
         <v>8770781.6251299996</v>
       </c>
-      <c r="L14" s="25">
-        <v>25</v>
-      </c>
-      <c r="M14" s="25">
-        <v>8</v>
-      </c>
-      <c r="N14" s="25">
+      <c r="L14" s="22">
+        <v>25</v>
+      </c>
+      <c r="M14" s="22">
+        <v>8</v>
+      </c>
+      <c r="N14" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="19">
         <f t="shared" si="5"/>
         <v>350831.2650052</v>
       </c>
-      <c r="P14" s="22">
+      <c r="P14" s="19">
         <f>58310*R5</f>
         <v>43853.908125649999</v>
       </c>
-      <c r="T14" s="19">
+      <c r="T14" s="16">
         <v>320110</v>
       </c>
-      <c r="U14" s="20">
+      <c r="U14" s="17">
         <f t="shared" si="6"/>
         <v>2560880</v>
       </c>
-      <c r="V14" s="20">
+      <c r="V14" s="17">
         <f t="shared" si="7"/>
         <v>64022000</v>
       </c>
@@ -1522,36 +1528,36 @@
       <c r="J15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="22">
         <f t="shared" si="3"/>
         <v>31324220.089749999</v>
       </c>
-      <c r="L15" s="25">
-        <v>25</v>
-      </c>
-      <c r="M15" s="25">
-        <v>8</v>
-      </c>
-      <c r="N15" s="25">
+      <c r="L15" s="22">
+        <v>25</v>
+      </c>
+      <c r="M15" s="22">
+        <v>8</v>
+      </c>
+      <c r="N15" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="19">
         <f t="shared" si="5"/>
         <v>1252968.8035899999</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="19">
         <f>208250*R5</f>
         <v>156621.10044874999</v>
       </c>
-      <c r="T15" s="19">
+      <c r="T15" s="16">
         <v>320110</v>
       </c>
-      <c r="U15" s="20">
+      <c r="U15" s="17">
         <f t="shared" si="6"/>
         <v>2560880</v>
       </c>
-      <c r="V15" s="20">
+      <c r="V15" s="17">
         <f t="shared" si="7"/>
         <v>64022000</v>
       </c>
@@ -1584,36 +1590,36 @@
       <c r="J16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="22">
         <f t="shared" si="3"/>
         <v>37231073.020960003</v>
       </c>
-      <c r="L16" s="25">
-        <v>25</v>
-      </c>
-      <c r="M16" s="25">
-        <v>8</v>
-      </c>
-      <c r="N16" s="25">
+      <c r="L16" s="22">
+        <v>25</v>
+      </c>
+      <c r="M16" s="22">
+        <v>8</v>
+      </c>
+      <c r="N16" s="22">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="19">
         <f t="shared" si="5"/>
         <v>1489242.9208384</v>
       </c>
-      <c r="P16" s="22">
+      <c r="P16" s="19">
         <f>247520*R5</f>
         <v>186155.3651048</v>
       </c>
-      <c r="T16" s="19">
+      <c r="T16" s="16">
         <v>247520</v>
       </c>
-      <c r="U16" s="20">
+      <c r="U16" s="17">
         <f t="shared" si="6"/>
         <v>1980160</v>
       </c>
-      <c r="V16" s="20">
+      <c r="V16" s="17">
         <f t="shared" si="7"/>
         <v>49504000</v>
       </c>
@@ -1643,18 +1649,18 @@
         <f t="shared" si="2"/>
         <v>13000</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="17">
         <f>SUM(K4:K16)</f>
         <v>453932697.98632002</v>
       </c>
-      <c r="T17" s="19">
+      <c r="T17" s="16">
         <v>320110</v>
       </c>
-      <c r="U17" s="20">
+      <c r="U17" s="17">
         <f t="shared" si="6"/>
         <v>2560880</v>
       </c>
-      <c r="V17" s="20">
+      <c r="V17" s="17">
         <f t="shared" si="7"/>
         <v>64022000</v>
       </c>
@@ -1687,18 +1693,18 @@
       <c r="J18" s="10">
         <v>2723596188</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="23">
         <f>K17*6</f>
         <v>2723596187.9179201</v>
       </c>
-      <c r="T18" s="19">
+      <c r="T18" s="16">
         <v>320110</v>
       </c>
-      <c r="U18" s="20">
+      <c r="U18" s="17">
         <f t="shared" si="6"/>
         <v>2560880</v>
       </c>
-      <c r="V18" s="20">
+      <c r="V18" s="17">
         <f t="shared" si="7"/>
         <v>64022000</v>
       </c>
@@ -1728,14 +1734,14 @@
         <f t="shared" si="2"/>
         <v>11000</v>
       </c>
-      <c r="T19" s="19">
+      <c r="T19" s="16">
         <v>114240</v>
       </c>
-      <c r="U19" s="20">
+      <c r="U19" s="17">
         <f t="shared" si="6"/>
         <v>913920</v>
       </c>
-      <c r="V19" s="20">
+      <c r="V19" s="17">
         <f t="shared" si="7"/>
         <v>22848000</v>
       </c>
@@ -1765,14 +1771,14 @@
         <f t="shared" si="2"/>
         <v>8500</v>
       </c>
-      <c r="T20" s="19">
+      <c r="T20" s="16">
         <v>124950</v>
       </c>
-      <c r="U20" s="20">
+      <c r="U20" s="17">
         <f t="shared" si="6"/>
         <v>999600</v>
       </c>
-      <c r="V20" s="20">
+      <c r="V20" s="17">
         <f t="shared" si="7"/>
         <v>24990000</v>
       </c>
@@ -1802,14 +1808,14 @@
         <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="T21" s="19">
+      <c r="T21" s="16">
         <v>58310</v>
       </c>
-      <c r="U21" s="20">
+      <c r="U21" s="17">
         <f t="shared" si="6"/>
         <v>466480</v>
       </c>
-      <c r="V21" s="20">
+      <c r="V21" s="17">
         <f t="shared" si="7"/>
         <v>11662000</v>
       </c>
@@ -1839,20 +1845,20 @@
         <f t="shared" si="2"/>
         <v>25000</v>
       </c>
-      <c r="O22" s="18">
+      <c r="O22" s="15">
         <v>3621408000</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="20">
         <v>1</v>
       </c>
-      <c r="T22" s="19">
+      <c r="T22" s="16">
         <v>208250</v>
       </c>
-      <c r="U22" s="20">
+      <c r="U22" s="17">
         <f t="shared" si="6"/>
         <v>1666000</v>
       </c>
-      <c r="V22" s="20">
+      <c r="V22" s="17">
         <f t="shared" si="7"/>
         <v>41650000</v>
       </c>
@@ -1882,32 +1888,32 @@
         <f t="shared" si="2"/>
         <v>13000</v>
       </c>
-      <c r="O23" s="18">
+      <c r="O23" s="15">
         <v>2723596188</v>
       </c>
       <c r="P23" t="s">
         <v>50</v>
       </c>
-      <c r="T23" s="19">
+      <c r="T23" s="16">
         <v>247520</v>
       </c>
-      <c r="U23" s="20">
+      <c r="U23" s="17">
         <f t="shared" si="6"/>
         <v>1980160</v>
       </c>
-      <c r="V23" s="20">
+      <c r="V23" s="17">
         <f t="shared" si="7"/>
         <v>49504000</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="V24" s="20">
+      <c r="V24" s="17">
         <f>SUM(V11:V23)*6</f>
         <v>3621408000</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="O25" s="24">
+      <c r="O25" s="21">
         <f>O23*P22/O22</f>
         <v>0.7520821150226652</v>
       </c>

</xml_diff>